<commit_message>
change margin for lab 12 excel
</commit_message>
<xml_diff>
--- a/Day12Excel/Lab12.xlsx
+++ b/Day12Excel/Lab12.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDriveAugie\OneDrive - Augustana College\Study\MATH440\Day12Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MATH440\Day12Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D899F6F1-0FD4-4780-B073-BCEED508FCB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{69BFF666-3B79-4246-8EB5-46E9A849F946}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
@@ -80,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -275,6 +274,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -395,6 +395,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1397,7 +1398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9BF645-C04E-4596-9961-CF4EB414E3EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2210,21 +2211,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9637D97D-24B5-4946-A7FB-2CFB7168B190}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2973,15 +2976,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A27599EA-7190-4F38-BF6B-114135086D84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -3935,7 +3942,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="78" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>